<commit_message>
primeira tentativa de classificador
</commit_message>
<xml_diff>
--- a/snickers.xlsx
+++ b/snickers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Documents/CD_2019-P2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54089BD5-EE38-A547-961A-0B2FAFCBA422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19E78FB-B37C-B745-A2BB-7743FAE3E234}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1955,7 +1955,7 @@
   <dimension ref="A1:B301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>